<commit_message>
Added next and last caches up to 3 chars for lookahead and lookbehind
</commit_message>
<xml_diff>
--- a/algorithm.xlsx
+++ b/algorithm.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="97">
   <si>
     <t>#</t>
   </si>
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>List</t>
   </si>
   <si>
     <t>ListItem</t>
@@ -3255,10 +3252,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3267,7 +3264,7 @@
     <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -3281,7 +3278,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3296,10 +3293,14 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G2" t="e">
+        <f>2^D1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -3319,10 +3320,14 @@
         <v xml:space="preserve"> = 1 &lt;&lt; 1</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G16" si="0">2^D2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -3338,14 +3343,18 @@
         <v>2</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ref="E4:E16" si="0">" = 1 &lt;&lt; "&amp;D4</f>
+        <f t="shared" ref="E4:E16" si="1">" = 1 &lt;&lt; "&amp;D4</f>
         <v xml:space="preserve"> = 1 &lt;&lt; 2</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -3361,14 +3370,18 @@
         <v>3</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 3</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -3384,16 +3397,20 @@
         <v>4</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="str">
         <f>IF(E8&lt;&gt;"",E7&amp;",",E7)</f>
@@ -3407,16 +3424,20 @@
         <v>5</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 5</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="str">
         <f>IF(E9&lt;&gt;"",E8&amp;",",E8)</f>
@@ -3430,14 +3451,18 @@
         <v>6</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 6</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -3453,14 +3478,18 @@
         <v>7</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 7</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3476,16 +3505,20 @@
         <v>8</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 8</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" t="str">
         <f>IF(E12&lt;&gt;"",E11&amp;",",E11)</f>
@@ -3499,14 +3532,18 @@
         <v>9</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 9</v>
       </c>
       <c r="F11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -3522,14 +3559,18 @@
         <v>10</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 10</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3545,14 +3586,18 @@
         <v>11</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 11</v>
       </c>
       <c r="F13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -3568,20 +3613,24 @@
         <v>12</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 12</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
       <c r="B15" t="str">
         <f>IF(E16&lt;&gt;"",E15&amp;",",E15)</f>
-        <v xml:space="preserve"> = 1 &lt;&lt; 13,</v>
+        <v xml:space="preserve"> = 1 &lt;&lt; 13</v>
       </c>
       <c r="C15">
         <v>3</v>
@@ -3591,34 +3640,15 @@
         <v>13</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> = 1 &lt;&lt; 13</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" t="str">
-        <f>IF(E17&lt;&gt;"",E16&amp;",",E16)</f>
-        <v xml:space="preserve"> = 1 &lt;&lt; 14</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <f>D15+1</f>
-        <v>14</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> = 1 &lt;&lt; 14</v>
-      </c>
-      <c r="F16" t="s">
-        <v>90</v>
+        <v>96</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>4096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>